<commit_message>
Trends framework and team switch
</commit_message>
<xml_diff>
--- a/2023-24 Conditional Formatting Cards/5 Year Trends/Team 5 Year Trends.xlsx
+++ b/2023-24 Conditional Formatting Cards/5 Year Trends/Team 5 Year Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataAnalystProjects\2023-24 Conditional Formatting Cards\5 Year Trends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B442120-81FD-43AF-99F2-789A05D6843C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7CBB93-77D4-46DF-9928-EC79C8E744B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{352E7898-3703-4855-B873-731E4161DCC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{352E7898-3703-4855-B873-731E4161DCC0}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-20" sheetId="5" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="2021-22" sheetId="3" r:id="rId3"/>
     <sheet name="2022-23" sheetId="2" r:id="rId4"/>
     <sheet name="2023-24" sheetId="1" r:id="rId5"/>
-    <sheet name="Master Table" sheetId="6" r:id="rId6"/>
+    <sheet name="2024-25" sheetId="7" r:id="rId6"/>
+    <sheet name="Master Table" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="46">
   <si>
     <t>Team</t>
   </si>
@@ -179,6 +180,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Utah Hockey Club (Formerly Arizona Coyotes)</t>
   </si>
 </sst>
 </file>
@@ -1777,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53A67B4-D84F-4D05-8E44-7C41A4DAD3BB}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8921,11 +8925,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9317F252-BB7C-4B22-AE54-B2858769FA56}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB92215-22F3-4D5A-A710-375A7D0BC3FB}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="Q122" sqref="Q122"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8972,52 +8988,40 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>'[1]All strength team card math'!H2</f>
-        <v>Anaheim Ducks</v>
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
-        <f>'[1]All strength team card math'!Q2</f>
         <v>29</v>
       </c>
       <c r="C2">
-        <f>'[1]All strength team card math'!S2</f>
         <v>27</v>
       </c>
       <c r="D2">
-        <f>'[1]All strength team card math'!T2</f>
         <v>27</v>
       </c>
       <c r="E2">
-        <f>'[1]All strength team card math'!I2</f>
         <v>19</v>
       </c>
       <c r="F2">
-        <f>'[1]All strength team card math'!K2</f>
         <v>23</v>
       </c>
       <c r="G2">
-        <f>'[1]All strength team card math'!M2</f>
         <v>28</v>
       </c>
       <c r="H2">
-        <f>'[1]All strength team card math'!U2</f>
         <v>25</v>
       </c>
       <c r="I2">
-        <f>'[1]All strength team card math'!J2</f>
         <v>26</v>
       </c>
       <c r="J2">
-        <f>'[1]All strength team card math'!L2</f>
         <v>24</v>
       </c>
       <c r="K2">
-        <f>'[1]All strength team card math'!N2</f>
         <v>24</v>
       </c>
       <c r="L2">
-        <f>'[1]All strength team card math'!O2</f>
         <v>17</v>
       </c>
       <c r="M2">
@@ -9025,52 +9029,40 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>'[1]All strength team card math'!H3</f>
-        <v>Arizona Coyotes</v>
+      <c r="A3" t="s">
+        <v>45</v>
       </c>
       <c r="B3">
-        <f>'[1]All strength team card math'!Q3</f>
         <v>17</v>
       </c>
       <c r="C3">
-        <f>'[1]All strength team card math'!S3</f>
         <v>22</v>
       </c>
       <c r="D3">
-        <f>'[1]All strength team card math'!T3</f>
         <v>22</v>
       </c>
       <c r="E3">
-        <f>'[1]All strength team card math'!I3</f>
         <v>16</v>
       </c>
       <c r="F3">
-        <f>'[1]All strength team card math'!K3</f>
         <v>27</v>
       </c>
       <c r="G3">
-        <f>'[1]All strength team card math'!M3</f>
         <v>23</v>
       </c>
       <c r="H3">
-        <f>'[1]All strength team card math'!U3</f>
         <v>23</v>
       </c>
       <c r="I3">
-        <f>'[1]All strength team card math'!J3</f>
         <v>29</v>
       </c>
       <c r="J3">
-        <f>'[1]All strength team card math'!L3</f>
         <v>15</v>
       </c>
       <c r="K3">
-        <f>'[1]All strength team card math'!N3</f>
         <v>3</v>
       </c>
       <c r="L3">
-        <f>'[1]All strength team card math'!O3</f>
         <v>3</v>
       </c>
       <c r="M3">
@@ -9078,52 +9070,40 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>'[1]All strength team card math'!H4</f>
-        <v>Boston Bruins</v>
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="B4">
-        <f>'[1]All strength team card math'!Q4</f>
         <v>1</v>
       </c>
       <c r="C4">
-        <f>'[1]All strength team card math'!S4</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f>'[1]All strength team card math'!T4</f>
         <v>11</v>
       </c>
       <c r="E4">
-        <f>'[1]All strength team card math'!I4</f>
         <v>10</v>
       </c>
       <c r="F4">
-        <f>'[1]All strength team card math'!K4</f>
         <v>17</v>
       </c>
       <c r="G4">
-        <f>'[1]All strength team card math'!M4</f>
         <v>9</v>
       </c>
       <c r="H4">
-        <f>'[1]All strength team card math'!U4</f>
         <v>5</v>
       </c>
       <c r="I4">
-        <f>'[1]All strength team card math'!J4</f>
         <v>9</v>
       </c>
       <c r="J4">
-        <f>'[1]All strength team card math'!L4</f>
         <v>3</v>
       </c>
       <c r="K4">
-        <f>'[1]All strength team card math'!N4</f>
         <v>1</v>
       </c>
       <c r="L4">
-        <f>'[1]All strength team card math'!O4</f>
         <v>2</v>
       </c>
       <c r="M4">
@@ -9131,52 +9111,40 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>'[1]All strength team card math'!H5</f>
-        <v>Buffalo Sabres</v>
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5">
-        <f>'[1]All strength team card math'!Q5</f>
         <v>27</v>
       </c>
       <c r="C5">
-        <f>'[1]All strength team card math'!S5</f>
         <v>25</v>
       </c>
       <c r="D5">
-        <f>'[1]All strength team card math'!T5</f>
         <v>30</v>
       </c>
       <c r="E5">
-        <f>'[1]All strength team card math'!I5</f>
         <v>28</v>
       </c>
       <c r="F5">
-        <f>'[1]All strength team card math'!K5</f>
         <v>30</v>
       </c>
       <c r="G5">
-        <f>'[1]All strength team card math'!M5</f>
         <v>21</v>
       </c>
       <c r="H5">
-        <f>'[1]All strength team card math'!U5</f>
         <v>14</v>
       </c>
       <c r="I5">
-        <f>'[1]All strength team card math'!J5</f>
         <v>15</v>
       </c>
       <c r="J5">
-        <f>'[1]All strength team card math'!L5</f>
         <v>12</v>
       </c>
       <c r="K5">
-        <f>'[1]All strength team card math'!N5</f>
         <v>22</v>
       </c>
       <c r="L5">
-        <f>'[1]All strength team card math'!O5</f>
         <v>26</v>
       </c>
       <c r="M5">
@@ -9184,52 +9152,40 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>'[1]All strength team card math'!H6</f>
-        <v>Calgary Flames</v>
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
-        <f>'[1]All strength team card math'!Q6</f>
         <v>16</v>
       </c>
       <c r="C6">
-        <f>'[1]All strength team card math'!S6</f>
         <v>18</v>
       </c>
       <c r="D6">
-        <f>'[1]All strength team card math'!T6</f>
         <v>11</v>
       </c>
       <c r="E6">
-        <f>'[1]All strength team card math'!I6</f>
         <v>8</v>
       </c>
       <c r="F6">
-        <f>'[1]All strength team card math'!K6</f>
         <v>8</v>
       </c>
       <c r="G6">
-        <f>'[1]All strength team card math'!M6</f>
         <v>20</v>
       </c>
       <c r="H6">
-        <f>'[1]All strength team card math'!U6</f>
         <v>24</v>
       </c>
       <c r="I6">
-        <f>'[1]All strength team card math'!J6</f>
         <v>27</v>
       </c>
       <c r="J6">
-        <f>'[1]All strength team card math'!L6</f>
         <v>20</v>
       </c>
       <c r="K6">
-        <f>'[1]All strength team card math'!N6</f>
         <v>16</v>
       </c>
       <c r="L6">
-        <f>'[1]All strength team card math'!O6</f>
         <v>15</v>
       </c>
       <c r="M6">
@@ -9237,52 +9193,40 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>'[1]All strength team card math'!H7</f>
-        <v>Carolina Hurricanes</v>
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
       <c r="B7">
-        <f>'[1]All strength team card math'!Q7</f>
         <v>5</v>
       </c>
       <c r="C7">
-        <f>'[1]All strength team card math'!S7</f>
         <v>9</v>
       </c>
       <c r="D7">
-        <f>'[1]All strength team card math'!T7</f>
         <v>4</v>
       </c>
       <c r="E7">
-        <f>'[1]All strength team card math'!I7</f>
         <v>5</v>
       </c>
       <c r="F7">
-        <f>'[1]All strength team card math'!K7</f>
         <v>1</v>
       </c>
       <c r="G7">
-        <f>'[1]All strength team card math'!M7</f>
         <v>11</v>
       </c>
       <c r="H7">
-        <f>'[1]All strength team card math'!U7</f>
         <v>12</v>
       </c>
       <c r="I7">
-        <f>'[1]All strength team card math'!J7</f>
         <v>4</v>
       </c>
       <c r="J7">
-        <f>'[1]All strength team card math'!L7</f>
         <v>21</v>
       </c>
       <c r="K7">
-        <f>'[1]All strength team card math'!N7</f>
         <v>10</v>
       </c>
       <c r="L7">
-        <f>'[1]All strength team card math'!O7</f>
         <v>12</v>
       </c>
       <c r="M7">
@@ -9290,52 +9234,40 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>'[1]All strength team card math'!H8</f>
-        <v>Chicago Blackhawks</v>
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8">
-        <f>'[1]All strength team card math'!Q8</f>
         <v>22</v>
       </c>
       <c r="C8">
-        <f>'[1]All strength team card math'!S8</f>
         <v>23</v>
       </c>
       <c r="D8">
-        <f>'[1]All strength team card math'!T8</f>
         <v>18</v>
       </c>
       <c r="E8">
-        <f>'[1]All strength team card math'!I8</f>
         <v>21</v>
       </c>
       <c r="F8">
-        <f>'[1]All strength team card math'!K8</f>
         <v>14</v>
       </c>
       <c r="G8">
-        <f>'[1]All strength team card math'!M8</f>
         <v>18</v>
       </c>
       <c r="H8">
-        <f>'[1]All strength team card math'!U8</f>
         <v>28</v>
       </c>
       <c r="I8">
-        <f>'[1]All strength team card math'!J8</f>
         <v>25</v>
       </c>
       <c r="J8">
-        <f>'[1]All strength team card math'!L8</f>
         <v>29</v>
       </c>
       <c r="K8">
-        <f>'[1]All strength team card math'!N8</f>
         <v>17</v>
       </c>
       <c r="L8">
-        <f>'[1]All strength team card math'!O8</f>
         <v>6</v>
       </c>
       <c r="M8">
@@ -9343,52 +9275,40 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>'[1]All strength team card math'!H9</f>
-        <v>Colorado Avalanche</v>
+      <c r="A9" t="s">
+        <v>19</v>
       </c>
       <c r="B9">
-        <f>'[1]All strength team card math'!Q9</f>
         <v>3</v>
       </c>
       <c r="C9">
-        <f>'[1]All strength team card math'!S9</f>
         <v>3</v>
       </c>
       <c r="D9">
-        <f>'[1]All strength team card math'!T9</f>
         <v>7</v>
       </c>
       <c r="E9">
-        <f>'[1]All strength team card math'!I9</f>
         <v>9</v>
       </c>
       <c r="F9">
-        <f>'[1]All strength team card math'!K9</f>
         <v>16</v>
       </c>
       <c r="G9">
-        <f>'[1]All strength team card math'!M9</f>
         <v>3</v>
       </c>
       <c r="H9">
-        <f>'[1]All strength team card math'!U9</f>
         <v>9</v>
       </c>
       <c r="I9">
-        <f>'[1]All strength team card math'!J9</f>
         <v>14</v>
       </c>
       <c r="J9">
-        <f>'[1]All strength team card math'!L9</f>
         <v>6</v>
       </c>
       <c r="K9">
-        <f>'[1]All strength team card math'!N9</f>
         <v>6</v>
       </c>
       <c r="L9">
-        <f>'[1]All strength team card math'!O9</f>
         <v>7</v>
       </c>
       <c r="M9">
@@ -9396,52 +9316,40 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f>'[1]All strength team card math'!H10</f>
-        <v>Columbus Blue Jackets</v>
+      <c r="A10" t="s">
+        <v>20</v>
       </c>
       <c r="B10">
-        <f>'[1]All strength team card math'!Q10</f>
         <v>13</v>
       </c>
       <c r="C10">
-        <f>'[1]All strength team card math'!S10</f>
         <v>13</v>
       </c>
       <c r="D10">
-        <f>'[1]All strength team card math'!T10</f>
         <v>28</v>
       </c>
       <c r="E10">
-        <f>'[1]All strength team card math'!I10</f>
         <v>20</v>
       </c>
       <c r="F10">
-        <f>'[1]All strength team card math'!K10</f>
         <v>28</v>
       </c>
       <c r="G10">
-        <f>'[1]All strength team card math'!M10</f>
         <v>28</v>
       </c>
       <c r="H10">
-        <f>'[1]All strength team card math'!U10</f>
         <v>3</v>
       </c>
       <c r="I10">
-        <f>'[1]All strength team card math'!J10</f>
         <v>6</v>
       </c>
       <c r="J10">
-        <f>'[1]All strength team card math'!L10</f>
         <v>1</v>
       </c>
       <c r="K10">
-        <f>'[1]All strength team card math'!N10</f>
         <v>3</v>
       </c>
       <c r="L10">
-        <f>'[1]All strength team card math'!O10</f>
         <v>12</v>
       </c>
       <c r="M10">
@@ -9449,52 +9357,40 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>'[1]All strength team card math'!H11</f>
-        <v>Dallas Stars</v>
+      <c r="A11" t="s">
+        <v>21</v>
       </c>
       <c r="B11">
-        <f>'[1]All strength team card math'!Q11</f>
         <v>9</v>
       </c>
       <c r="C11">
-        <f>'[1]All strength team card math'!S11</f>
         <v>10</v>
       </c>
       <c r="D11">
-        <f>'[1]All strength team card math'!T11</f>
         <v>21</v>
       </c>
       <c r="E11">
-        <f>'[1]All strength team card math'!I11</f>
         <v>24</v>
       </c>
       <c r="F11">
-        <f>'[1]All strength team card math'!K11</f>
         <v>12</v>
       </c>
       <c r="G11">
-        <f>'[1]All strength team card math'!M11</f>
         <v>26</v>
       </c>
       <c r="H11">
-        <f>'[1]All strength team card math'!U11</f>
         <v>13</v>
       </c>
       <c r="I11">
-        <f>'[1]All strength team card math'!J11</f>
         <v>16</v>
       </c>
       <c r="J11">
-        <f>'[1]All strength team card math'!L11</f>
         <v>10</v>
       </c>
       <c r="K11">
-        <f>'[1]All strength team card math'!N11</f>
         <v>2</v>
       </c>
       <c r="L11">
-        <f>'[1]All strength team card math'!O11</f>
         <v>1</v>
       </c>
       <c r="M11">
@@ -9502,52 +9398,40 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f>'[1]All strength team card math'!H12</f>
-        <v>Detroit Red Wings</v>
+      <c r="A12" t="s">
+        <v>22</v>
       </c>
       <c r="B12">
-        <f>'[1]All strength team card math'!Q12</f>
         <v>31</v>
       </c>
       <c r="C12">
-        <f>'[1]All strength team card math'!S12</f>
         <v>31</v>
       </c>
       <c r="D12">
-        <f>'[1]All strength team card math'!T12</f>
         <v>31</v>
       </c>
       <c r="E12">
-        <f>'[1]All strength team card math'!I12</f>
         <v>31</v>
       </c>
       <c r="F12">
-        <f>'[1]All strength team card math'!K12</f>
         <v>31</v>
       </c>
       <c r="G12">
-        <f>'[1]All strength team card math'!M12</f>
         <v>31</v>
       </c>
       <c r="H12">
-        <f>'[1]All strength team card math'!U12</f>
         <v>27</v>
       </c>
       <c r="I12">
-        <f>'[1]All strength team card math'!J12</f>
         <v>23</v>
       </c>
       <c r="J12">
-        <f>'[1]All strength team card math'!L12</f>
         <v>30</v>
       </c>
       <c r="K12">
-        <f>'[1]All strength team card math'!N12</f>
         <v>31</v>
       </c>
       <c r="L12">
-        <f>'[1]All strength team card math'!O12</f>
         <v>31</v>
       </c>
       <c r="M12">
@@ -9555,52 +9439,40 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f>'[1]All strength team card math'!H13</f>
-        <v>Edmonton Oilers</v>
+      <c r="A13" t="s">
+        <v>23</v>
       </c>
       <c r="B13">
-        <f>'[1]All strength team card math'!Q13</f>
         <v>23</v>
       </c>
       <c r="C13">
-        <f>'[1]All strength team card math'!S13</f>
         <v>12</v>
       </c>
       <c r="D13">
-        <f>'[1]All strength team card math'!T13</f>
         <v>20</v>
       </c>
       <c r="E13">
-        <f>'[1]All strength team card math'!I13</f>
         <v>29</v>
       </c>
       <c r="F13">
-        <f>'[1]All strength team card math'!K13</f>
         <v>18</v>
       </c>
       <c r="G13">
-        <f>'[1]All strength team card math'!M13</f>
         <v>14</v>
       </c>
       <c r="H13">
-        <f>'[1]All strength team card math'!U13</f>
         <v>20</v>
       </c>
       <c r="I13">
-        <f>'[1]All strength team card math'!J13</f>
         <v>19</v>
       </c>
       <c r="J13">
-        <f>'[1]All strength team card math'!L13</f>
         <v>22</v>
       </c>
       <c r="K13">
-        <f>'[1]All strength team card math'!N13</f>
         <v>15</v>
       </c>
       <c r="L13">
-        <f>'[1]All strength team card math'!O13</f>
         <v>14</v>
       </c>
       <c r="M13">
@@ -9608,52 +9480,40 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f>'[1]All strength team card math'!H14</f>
-        <v>Florida Panthers</v>
+      <c r="A14" t="s">
+        <v>24</v>
       </c>
       <c r="B14">
-        <f>'[1]All strength team card math'!Q14</f>
         <v>25</v>
       </c>
       <c r="C14">
-        <f>'[1]All strength team card math'!S14</f>
         <v>15</v>
       </c>
       <c r="D14">
-        <f>'[1]All strength team card math'!T14</f>
         <v>13</v>
       </c>
       <c r="E14">
-        <f>'[1]All strength team card math'!I14</f>
         <v>11</v>
       </c>
       <c r="F14">
-        <f>'[1]All strength team card math'!K14</f>
         <v>20</v>
       </c>
       <c r="G14">
-        <f>'[1]All strength team card math'!M14</f>
         <v>6</v>
       </c>
       <c r="H14">
-        <f>'[1]All strength team card math'!U14</f>
         <v>20</v>
       </c>
       <c r="I14">
-        <f>'[1]All strength team card math'!J14</f>
         <v>18</v>
       </c>
       <c r="J14">
-        <f>'[1]All strength team card math'!L14</f>
         <v>23</v>
       </c>
       <c r="K14">
-        <f>'[1]All strength team card math'!N14</f>
         <v>29</v>
       </c>
       <c r="L14">
-        <f>'[1]All strength team card math'!O14</f>
         <v>28</v>
       </c>
       <c r="M14">
@@ -9661,52 +9521,40 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f>'[1]All strength team card math'!H15</f>
-        <v>Los Angeles Kings</v>
+      <c r="A15" t="s">
+        <v>25</v>
       </c>
       <c r="B15">
-        <f>'[1]All strength team card math'!Q15</f>
         <v>15</v>
       </c>
       <c r="C15">
-        <f>'[1]All strength team card math'!S15</f>
         <v>28</v>
       </c>
       <c r="D15">
-        <f>'[1]All strength team card math'!T15</f>
         <v>14</v>
       </c>
       <c r="E15">
-        <f>'[1]All strength team card math'!I15</f>
         <v>2</v>
       </c>
       <c r="F15">
-        <f>'[1]All strength team card math'!K15</f>
         <v>8</v>
       </c>
       <c r="G15">
-        <f>'[1]All strength team card math'!M15</f>
         <v>30</v>
       </c>
       <c r="H15">
-        <f>'[1]All strength team card math'!U15</f>
         <v>15</v>
       </c>
       <c r="I15">
-        <f>'[1]All strength team card math'!J15</f>
         <v>10</v>
       </c>
       <c r="J15">
-        <f>'[1]All strength team card math'!L15</f>
         <v>18</v>
       </c>
       <c r="K15">
-        <f>'[1]All strength team card math'!N15</f>
         <v>14</v>
       </c>
       <c r="L15">
-        <f>'[1]All strength team card math'!O15</f>
         <v>19</v>
       </c>
       <c r="M15">
@@ -9714,52 +9562,40 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <f>'[1]All strength team card math'!H16</f>
-        <v>Minnesota Wild</v>
+      <c r="A16" t="s">
+        <v>26</v>
       </c>
       <c r="B16">
-        <f>'[1]All strength team card math'!Q16</f>
         <v>24</v>
       </c>
       <c r="C16">
-        <f>'[1]All strength team card math'!S16</f>
         <v>21</v>
       </c>
       <c r="D16">
-        <f>'[1]All strength team card math'!T16</f>
         <v>22</v>
       </c>
       <c r="E16">
-        <f>'[1]All strength team card math'!I16</f>
         <v>25</v>
       </c>
       <c r="F16">
-        <f>'[1]All strength team card math'!K16</f>
         <v>29</v>
       </c>
       <c r="G16">
-        <f>'[1]All strength team card math'!M16</f>
         <v>12</v>
       </c>
       <c r="H16">
-        <f>'[1]All strength team card math'!U16</f>
         <v>6</v>
       </c>
       <c r="I16">
-        <f>'[1]All strength team card math'!J16</f>
         <v>13</v>
       </c>
       <c r="J16">
-        <f>'[1]All strength team card math'!L16</f>
         <v>2</v>
       </c>
       <c r="K16">
-        <f>'[1]All strength team card math'!N16</f>
         <v>23</v>
       </c>
       <c r="L16">
-        <f>'[1]All strength team card math'!O16</f>
         <v>30</v>
       </c>
       <c r="M16">
@@ -9767,52 +9603,40 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <f>'[1]All strength team card math'!H17</f>
-        <v>Montreal Canadiens</v>
+      <c r="A17" t="s">
+        <v>27</v>
       </c>
       <c r="B17">
-        <f>'[1]All strength team card math'!Q17</f>
         <v>11</v>
       </c>
       <c r="C17">
-        <f>'[1]All strength team card math'!S17</f>
         <v>24</v>
       </c>
       <c r="D17">
-        <f>'[1]All strength team card math'!T17</f>
         <v>8</v>
       </c>
       <c r="E17">
-        <f>'[1]All strength team card math'!I17</f>
         <v>3</v>
       </c>
       <c r="F17">
-        <f>'[1]All strength team card math'!K17</f>
         <v>8</v>
       </c>
       <c r="G17">
-        <f>'[1]All strength team card math'!M17</f>
         <v>19</v>
       </c>
       <c r="H17">
-        <f>'[1]All strength team card math'!U17</f>
         <v>9</v>
       </c>
       <c r="I17">
-        <f>'[1]All strength team card math'!J17</f>
         <v>12</v>
       </c>
       <c r="J17">
-        <f>'[1]All strength team card math'!L17</f>
         <v>8</v>
       </c>
       <c r="K17">
-        <f>'[1]All strength team card math'!N17</f>
         <v>19</v>
       </c>
       <c r="L17">
-        <f>'[1]All strength team card math'!O17</f>
         <v>26</v>
       </c>
       <c r="M17">
@@ -9820,52 +9644,40 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <f>'[1]All strength team card math'!H18</f>
-        <v>Nashville Predators</v>
+      <c r="A18" t="s">
+        <v>28</v>
       </c>
       <c r="B18">
-        <f>'[1]All strength team card math'!Q18</f>
         <v>10</v>
       </c>
       <c r="C18">
-        <f>'[1]All strength team card math'!S18</f>
         <v>15</v>
       </c>
       <c r="D18">
-        <f>'[1]All strength team card math'!T18</f>
         <v>6</v>
       </c>
       <c r="E18">
-        <f>'[1]All strength team card math'!I18</f>
         <v>4</v>
       </c>
       <c r="F18">
-        <f>'[1]All strength team card math'!K18</f>
         <v>5</v>
       </c>
       <c r="G18">
-        <f>'[1]All strength team card math'!M18</f>
         <v>16</v>
       </c>
       <c r="H18">
-        <f>'[1]All strength team card math'!U18</f>
         <v>15</v>
       </c>
       <c r="I18">
-        <f>'[1]All strength team card math'!J18</f>
         <v>17</v>
       </c>
       <c r="J18">
-        <f>'[1]All strength team card math'!L18</f>
         <v>11</v>
       </c>
       <c r="K18">
-        <f>'[1]All strength team card math'!N18</f>
         <v>19</v>
       </c>
       <c r="L18">
-        <f>'[1]All strength team card math'!O18</f>
         <v>20</v>
       </c>
       <c r="M18">
@@ -9873,52 +9685,40 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <f>'[1]All strength team card math'!H19</f>
-        <v>New Jersey Devils</v>
+      <c r="A19" t="s">
+        <v>29</v>
       </c>
       <c r="B19">
-        <f>'[1]All strength team card math'!Q19</f>
         <v>29</v>
       </c>
       <c r="C19">
-        <f>'[1]All strength team card math'!S19</f>
         <v>25</v>
       </c>
       <c r="D19">
-        <f>'[1]All strength team card math'!T19</f>
         <v>24</v>
       </c>
       <c r="E19">
-        <f>'[1]All strength team card math'!I19</f>
         <v>23</v>
       </c>
       <c r="F19">
-        <f>'[1]All strength team card math'!K19</f>
         <v>20</v>
       </c>
       <c r="G19">
-        <f>'[1]All strength team card math'!M19</f>
         <v>24</v>
       </c>
       <c r="H19">
-        <f>'[1]All strength team card math'!U19</f>
         <v>22</v>
       </c>
       <c r="I19">
-        <f>'[1]All strength team card math'!J19</f>
         <v>24</v>
       </c>
       <c r="J19">
-        <f>'[1]All strength team card math'!L19</f>
         <v>18</v>
       </c>
       <c r="K19">
-        <f>'[1]All strength team card math'!N19</f>
         <v>28</v>
       </c>
       <c r="L19">
-        <f>'[1]All strength team card math'!O19</f>
         <v>24</v>
       </c>
       <c r="M19">
@@ -9926,52 +9726,40 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <f>'[1]All strength team card math'!H20</f>
-        <v>New York Islanders</v>
+      <c r="A20" t="s">
+        <v>30</v>
       </c>
       <c r="B20">
-        <f>'[1]All strength team card math'!Q20</f>
         <v>21</v>
       </c>
       <c r="C20">
-        <f>'[1]All strength team card math'!S20</f>
         <v>11</v>
       </c>
       <c r="D20">
-        <f>'[1]All strength team card math'!T20</f>
         <v>28</v>
       </c>
       <c r="E20">
-        <f>'[1]All strength team card math'!I20</f>
         <v>30</v>
       </c>
       <c r="F20">
-        <f>'[1]All strength team card math'!K20</f>
         <v>24</v>
       </c>
       <c r="G20">
-        <f>'[1]All strength team card math'!M20</f>
         <v>22</v>
       </c>
       <c r="H20">
-        <f>'[1]All strength team card math'!U20</f>
         <v>17</v>
       </c>
       <c r="I20">
-        <f>'[1]All strength team card math'!J20</f>
         <v>21</v>
       </c>
       <c r="J20">
-        <f>'[1]All strength team card math'!L20</f>
         <v>12</v>
       </c>
       <c r="K20">
-        <f>'[1]All strength team card math'!N20</f>
         <v>9</v>
       </c>
       <c r="L20">
-        <f>'[1]All strength team card math'!O20</f>
         <v>9</v>
       </c>
       <c r="M20">
@@ -9979,52 +9767,40 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f>'[1]All strength team card math'!H21</f>
-        <v>New York Rangers</v>
+      <c r="A21" t="s">
+        <v>31</v>
       </c>
       <c r="B21">
-        <f>'[1]All strength team card math'!Q21</f>
         <v>20</v>
       </c>
       <c r="C21">
-        <f>'[1]All strength team card math'!S21</f>
         <v>18</v>
       </c>
       <c r="D21">
-        <f>'[1]All strength team card math'!T21</f>
         <v>10</v>
       </c>
       <c r="E21">
-        <f>'[1]All strength team card math'!I21</f>
         <v>18</v>
       </c>
       <c r="F21">
-        <f>'[1]All strength team card math'!K21</f>
         <v>12</v>
       </c>
       <c r="G21">
-        <f>'[1]All strength team card math'!M21</f>
         <v>5</v>
       </c>
       <c r="H21">
-        <f>'[1]All strength team card math'!U21</f>
         <v>31</v>
       </c>
       <c r="I21">
-        <f>'[1]All strength team card math'!J21</f>
         <v>31</v>
       </c>
       <c r="J21">
-        <f>'[1]All strength team card math'!L21</f>
         <v>31</v>
       </c>
       <c r="K21">
-        <f>'[1]All strength team card math'!N21</f>
         <v>24</v>
       </c>
       <c r="L21">
-        <f>'[1]All strength team card math'!O21</f>
         <v>5</v>
       </c>
       <c r="M21">
@@ -10032,52 +9808,40 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <f>'[1]All strength team card math'!H22</f>
-        <v>Ottawa Senators</v>
+      <c r="A22" t="s">
+        <v>32</v>
       </c>
       <c r="B22">
-        <f>'[1]All strength team card math'!Q22</f>
         <v>26</v>
       </c>
       <c r="C22">
-        <f>'[1]All strength team card math'!S22</f>
         <v>30</v>
       </c>
       <c r="D22">
-        <f>'[1]All strength team card math'!T22</f>
         <v>16</v>
       </c>
       <c r="E22">
-        <f>'[1]All strength team card math'!I22</f>
         <v>13</v>
       </c>
       <c r="F22">
-        <f>'[1]All strength team card math'!K22</f>
         <v>8</v>
       </c>
       <c r="G22">
-        <f>'[1]All strength team card math'!M22</f>
         <v>24</v>
       </c>
       <c r="H22">
-        <f>'[1]All strength team card math'!U22</f>
         <v>30</v>
       </c>
       <c r="I22">
-        <f>'[1]All strength team card math'!J22</f>
         <v>30</v>
       </c>
       <c r="J22">
-        <f>'[1]All strength team card math'!L22</f>
         <v>26</v>
       </c>
       <c r="K22">
-        <f>'[1]All strength team card math'!N22</f>
         <v>30</v>
       </c>
       <c r="L22">
-        <f>'[1]All strength team card math'!O22</f>
         <v>22</v>
       </c>
       <c r="M22">
@@ -10085,52 +9849,40 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <f>'[1]All strength team card math'!H23</f>
-        <v>Philadelphia Flyers</v>
+      <c r="A23" t="s">
+        <v>33</v>
       </c>
       <c r="B23">
-        <f>'[1]All strength team card math'!Q23</f>
         <v>8</v>
       </c>
       <c r="C23">
-        <f>'[1]All strength team card math'!S23</f>
         <v>6</v>
       </c>
       <c r="D23">
-        <f>'[1]All strength team card math'!T23</f>
         <v>17</v>
       </c>
       <c r="E23">
-        <f>'[1]All strength team card math'!I23</f>
         <v>21</v>
       </c>
       <c r="F23">
-        <f>'[1]All strength team card math'!K23</f>
         <v>22</v>
       </c>
       <c r="G23">
-        <f>'[1]All strength team card math'!M23</f>
         <v>7</v>
       </c>
       <c r="H23">
-        <f>'[1]All strength team card math'!U23</f>
         <v>1</v>
       </c>
       <c r="I23">
-        <f>'[1]All strength team card math'!J23</f>
         <v>1</v>
       </c>
       <c r="J23">
-        <f>'[1]All strength team card math'!L23</f>
         <v>5</v>
       </c>
       <c r="K23">
-        <f>'[1]All strength team card math'!N23</f>
         <v>7</v>
       </c>
       <c r="L23">
-        <f>'[1]All strength team card math'!O23</f>
         <v>15</v>
       </c>
       <c r="M23">
@@ -10138,52 +9890,40 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <f>'[1]All strength team card math'!H24</f>
-        <v>Pittsburgh Penguins</v>
+      <c r="A24" t="s">
+        <v>34</v>
       </c>
       <c r="B24">
-        <f>'[1]All strength team card math'!Q24</f>
         <v>6</v>
       </c>
       <c r="C24">
-        <f>'[1]All strength team card math'!S24</f>
         <v>7</v>
       </c>
       <c r="D24">
-        <f>'[1]All strength team card math'!T24</f>
         <v>9</v>
       </c>
       <c r="E24">
-        <f>'[1]All strength team card math'!I24</f>
         <v>17</v>
       </c>
       <c r="F24">
-        <f>'[1]All strength team card math'!K24</f>
         <v>5</v>
       </c>
       <c r="G24">
-        <f>'[1]All strength team card math'!M24</f>
         <v>10</v>
       </c>
       <c r="H24">
-        <f>'[1]All strength team card math'!U24</f>
         <v>1</v>
       </c>
       <c r="I24">
-        <f>'[1]All strength team card math'!J24</f>
         <v>2</v>
       </c>
       <c r="J24">
-        <f>'[1]All strength team card math'!L24</f>
         <v>4</v>
       </c>
       <c r="K24">
-        <f>'[1]All strength team card math'!N24</f>
         <v>10</v>
       </c>
       <c r="L24">
-        <f>'[1]All strength team card math'!O24</f>
         <v>18</v>
       </c>
       <c r="M24">
@@ -10191,52 +9931,40 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <f>'[1]All strength team card math'!H25</f>
-        <v>San Jose Sharks</v>
+      <c r="A25" t="s">
+        <v>35</v>
       </c>
       <c r="B25">
-        <f>'[1]All strength team card math'!Q25</f>
         <v>28</v>
       </c>
       <c r="C25">
-        <f>'[1]All strength team card math'!S25</f>
         <v>29</v>
       </c>
       <c r="D25">
-        <f>'[1]All strength team card math'!T25</f>
         <v>24</v>
       </c>
       <c r="E25">
-        <f>'[1]All strength team card math'!I25</f>
         <v>26</v>
       </c>
       <c r="F25">
-        <f>'[1]All strength team card math'!K25</f>
         <v>15</v>
       </c>
       <c r="G25">
-        <f>'[1]All strength team card math'!M25</f>
         <v>26</v>
       </c>
       <c r="H25">
-        <f>'[1]All strength team card math'!U25</f>
         <v>18</v>
       </c>
       <c r="I25">
-        <f>'[1]All strength team card math'!J25</f>
         <v>11</v>
       </c>
       <c r="J25">
-        <f>'[1]All strength team card math'!L25</f>
         <v>25</v>
       </c>
       <c r="K25">
-        <f>'[1]All strength team card math'!N25</f>
         <v>27</v>
       </c>
       <c r="L25">
-        <f>'[1]All strength team card math'!O25</f>
         <v>28</v>
       </c>
       <c r="M25">
@@ -10252,52 +9980,40 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <f>'[1]All strength team card math'!H26</f>
-        <v>St Louis Blues</v>
+      <c r="A27" t="s">
+        <v>37</v>
       </c>
       <c r="B27">
-        <f>'[1]All strength team card math'!Q26</f>
         <v>12</v>
       </c>
       <c r="C27">
-        <f>'[1]All strength team card math'!S26</f>
         <v>2</v>
       </c>
       <c r="D27">
-        <f>'[1]All strength team card math'!T26</f>
         <v>24</v>
       </c>
       <c r="E27">
-        <f>'[1]All strength team card math'!I26</f>
         <v>27</v>
       </c>
       <c r="F27">
-        <f>'[1]All strength team card math'!K26</f>
         <v>25</v>
       </c>
       <c r="G27">
-        <f>'[1]All strength team card math'!M26</f>
         <v>15</v>
       </c>
       <c r="H27">
-        <f>'[1]All strength team card math'!U26</f>
         <v>8</v>
       </c>
       <c r="I27">
-        <f>'[1]All strength team card math'!J26</f>
         <v>5</v>
       </c>
       <c r="J27">
-        <f>'[1]All strength team card math'!L26</f>
         <v>12</v>
       </c>
       <c r="K27">
-        <f>'[1]All strength team card math'!N26</f>
         <v>5</v>
       </c>
       <c r="L27">
-        <f>'[1]All strength team card math'!O26</f>
         <v>8</v>
       </c>
       <c r="M27">
@@ -10305,52 +10021,40 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <f>'[1]All strength team card math'!H27</f>
-        <v>Tampa Bay Lightning</v>
+      <c r="A28" t="s">
+        <v>38</v>
       </c>
       <c r="B28">
-        <f>'[1]All strength team card math'!Q27</f>
         <v>2</v>
       </c>
       <c r="C28">
-        <f>'[1]All strength team card math'!S27</f>
         <v>3</v>
       </c>
       <c r="D28">
-        <f>'[1]All strength team card math'!T27</f>
         <v>5</v>
       </c>
       <c r="E28">
-        <f>'[1]All strength team card math'!I27</f>
         <v>12</v>
       </c>
       <c r="F28">
-        <f>'[1]All strength team card math'!K27</f>
         <v>7</v>
       </c>
       <c r="G28">
-        <f>'[1]All strength team card math'!M27</f>
         <v>1</v>
       </c>
       <c r="H28">
-        <f>'[1]All strength team card math'!U27</f>
         <v>6</v>
       </c>
       <c r="I28">
-        <f>'[1]All strength team card math'!J27</f>
         <v>8</v>
       </c>
       <c r="J28">
-        <f>'[1]All strength team card math'!L27</f>
         <v>7</v>
       </c>
       <c r="K28">
-        <f>'[1]All strength team card math'!N27</f>
         <v>8</v>
       </c>
       <c r="L28">
-        <f>'[1]All strength team card math'!O27</f>
         <v>10</v>
       </c>
       <c r="M28">
@@ -10358,52 +10062,40 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <f>'[1]All strength team card math'!H28</f>
-        <v>Toronto Maple Leafs</v>
+      <c r="A29" t="s">
+        <v>39</v>
       </c>
       <c r="B29">
-        <f>'[1]All strength team card math'!Q28</f>
         <v>14</v>
       </c>
       <c r="C29">
-        <f>'[1]All strength team card math'!S28</f>
         <v>13</v>
       </c>
       <c r="D29">
-        <f>'[1]All strength team card math'!T28</f>
         <v>2</v>
       </c>
       <c r="E29">
-        <f>'[1]All strength team card math'!I28</f>
         <v>6</v>
       </c>
       <c r="F29">
-        <f>'[1]All strength team card math'!K28</f>
         <v>4</v>
       </c>
       <c r="G29">
-        <f>'[1]All strength team card math'!M28</f>
         <v>3</v>
       </c>
       <c r="H29">
-        <f>'[1]All strength team card math'!U28</f>
         <v>18</v>
       </c>
       <c r="I29">
-        <f>'[1]All strength team card math'!J28</f>
         <v>20</v>
       </c>
       <c r="J29">
-        <f>'[1]All strength team card math'!L28</f>
         <v>16</v>
       </c>
       <c r="K29">
-        <f>'[1]All strength team card math'!N28</f>
         <v>26</v>
       </c>
       <c r="L29">
-        <f>'[1]All strength team card math'!O28</f>
         <v>24</v>
       </c>
       <c r="M29">
@@ -10411,52 +10103,40 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <f>'[1]All strength team card math'!H29</f>
-        <v>Vancouver Canucks</v>
+      <c r="A30" t="s">
+        <v>40</v>
       </c>
       <c r="B30">
-        <f>'[1]All strength team card math'!Q29</f>
         <v>18</v>
       </c>
       <c r="C30">
-        <f>'[1]All strength team card math'!S29</f>
         <v>15</v>
       </c>
       <c r="D30">
-        <f>'[1]All strength team card math'!T29</f>
         <v>15</v>
       </c>
       <c r="E30">
-        <f>'[1]All strength team card math'!I29</f>
         <v>14</v>
       </c>
       <c r="F30">
-        <f>'[1]All strength team card math'!K29</f>
         <v>19</v>
       </c>
       <c r="G30">
-        <f>'[1]All strength team card math'!M29</f>
         <v>8</v>
       </c>
       <c r="H30">
-        <f>'[1]All strength team card math'!U29</f>
         <v>25</v>
       </c>
       <c r="I30">
-        <f>'[1]All strength team card math'!J29</f>
         <v>22</v>
       </c>
       <c r="J30">
-        <f>'[1]All strength team card math'!L29</f>
         <v>28</v>
       </c>
       <c r="K30">
-        <f>'[1]All strength team card math'!N29</f>
         <v>21</v>
       </c>
       <c r="L30">
-        <f>'[1]All strength team card math'!O29</f>
         <v>10</v>
       </c>
       <c r="M30">
@@ -10464,52 +10144,40 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <f>'[1]All strength team card math'!H30</f>
-        <v>Vegas Golden Knights</v>
+      <c r="A31" t="s">
+        <v>41</v>
       </c>
       <c r="B31">
-        <f>'[1]All strength team card math'!Q30</f>
         <v>3</v>
       </c>
       <c r="C31">
-        <f>'[1]All strength team card math'!S30</f>
         <v>8</v>
       </c>
       <c r="D31">
-        <f>'[1]All strength team card math'!T30</f>
         <v>3</v>
       </c>
       <c r="E31">
-        <f>'[1]All strength team card math'!I30</f>
         <v>1</v>
       </c>
       <c r="F31">
-        <f>'[1]All strength team card math'!K30</f>
         <v>2</v>
       </c>
       <c r="G31">
-        <f>'[1]All strength team card math'!M30</f>
         <v>13</v>
       </c>
       <c r="H31">
-        <f>'[1]All strength team card math'!U30</f>
         <v>4</v>
       </c>
       <c r="I31">
-        <f>'[1]All strength team card math'!J30</f>
         <v>3</v>
       </c>
       <c r="J31">
-        <f>'[1]All strength team card math'!L30</f>
         <v>8</v>
       </c>
       <c r="K31">
-        <f>'[1]All strength team card math'!N30</f>
         <v>13</v>
       </c>
       <c r="L31">
-        <f>'[1]All strength team card math'!O30</f>
         <v>21</v>
       </c>
       <c r="M31">
@@ -10517,52 +10185,40 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f>'[1]All strength team card math'!H31</f>
-        <v>Washington Capitals</v>
+      <c r="A32" t="s">
+        <v>42</v>
       </c>
       <c r="B32">
-        <f>'[1]All strength team card math'!Q31</f>
         <v>7</v>
       </c>
       <c r="C32">
-        <f>'[1]All strength team card math'!S31</f>
         <v>5</v>
       </c>
       <c r="D32">
-        <f>'[1]All strength team card math'!T31</f>
         <v>1</v>
       </c>
       <c r="E32">
-        <f>'[1]All strength team card math'!I31</f>
         <v>7</v>
       </c>
       <c r="F32">
-        <f>'[1]All strength team card math'!K31</f>
         <v>3</v>
       </c>
       <c r="G32">
-        <f>'[1]All strength team card math'!M31</f>
         <v>2</v>
       </c>
       <c r="H32">
-        <f>'[1]All strength team card math'!U31</f>
         <v>11</v>
       </c>
       <c r="I32">
-        <f>'[1]All strength team card math'!J31</f>
         <v>7</v>
       </c>
       <c r="J32">
-        <f>'[1]All strength team card math'!L31</f>
         <v>17</v>
       </c>
       <c r="K32">
-        <f>'[1]All strength team card math'!N31</f>
         <v>18</v>
       </c>
       <c r="L32">
-        <f>'[1]All strength team card math'!O31</f>
         <v>23</v>
       </c>
       <c r="M32">
@@ -10570,52 +10226,40 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <f>'[1]All strength team card math'!H32</f>
-        <v>Winnipeg Jets</v>
+      <c r="A33" t="s">
+        <v>43</v>
       </c>
       <c r="B33">
-        <f>'[1]All strength team card math'!Q32</f>
         <v>19</v>
       </c>
       <c r="C33">
-        <f>'[1]All strength team card math'!S32</f>
         <v>20</v>
       </c>
       <c r="D33">
-        <f>'[1]All strength team card math'!T32</f>
         <v>19</v>
       </c>
       <c r="E33">
-        <f>'[1]All strength team card math'!I32</f>
         <v>15</v>
       </c>
       <c r="F33">
-        <f>'[1]All strength team card math'!K32</f>
         <v>25</v>
       </c>
       <c r="G33">
-        <f>'[1]All strength team card math'!M32</f>
         <v>17</v>
       </c>
       <c r="H33">
-        <f>'[1]All strength team card math'!U32</f>
         <v>29</v>
       </c>
       <c r="I33">
-        <f>'[1]All strength team card math'!J32</f>
         <v>28</v>
       </c>
       <c r="J33">
-        <f>'[1]All strength team card math'!L32</f>
         <v>27</v>
       </c>
       <c r="K33">
-        <f>'[1]All strength team card math'!N32</f>
         <v>10</v>
       </c>
       <c r="L33">
-        <f>'[1]All strength team card math'!O32</f>
         <v>3</v>
       </c>
       <c r="M33">
@@ -10665,7 +10309,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>23</v>
@@ -11944,7 +11588,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B67">
         <v>32</v>
@@ -13256,7 +12900,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B99">
         <v>28</v>
@@ -14568,7 +14212,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B131">
         <v>27</v>

</xml_diff>